<commit_message>
fixed notes column bc datasheet mistakes were fixed
also took new photos of datasheet
</commit_message>
<xml_diff>
--- a/Probiotics_Transmission_Data/COL_SAN_protran_sample_data.xlsx
+++ b/Probiotics_Transmission_Data/COL_SAN_protran_sample_data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikea_ulrich/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikea_ulrich/Documents/GitHub/SAN_CORDAP/Probiotics_Transmission_Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F95E2D5-BF9A-814F-9830-86C4DF11EA49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A50625B-568E-3545-AB57-E8B8679E0815}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4940" yWindow="800" windowWidth="23480" windowHeight="17120" xr2:uid="{4E2C8971-6FF9-7D4C-A5F6-9C03F4C73A1D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="780" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="25">
   <si>
     <t>species</t>
   </si>
@@ -111,57 +111,6 @@
   </si>
   <si>
     <t>pale on top</t>
-  </si>
-  <si>
-    <t>data sheet says genet 001, but should be genet 031</t>
-  </si>
-  <si>
-    <t>data sheet says genet 029, but it is genet 293</t>
-  </si>
-  <si>
-    <t>data sheet says genet 029, but it is genet 294</t>
-  </si>
-  <si>
-    <t>data sheet says genet 029, but it is genet 295</t>
-  </si>
-  <si>
-    <t>data sheet says genet 029, but it is genet 296</t>
-  </si>
-  <si>
-    <t>data sheet says genet 029, but it is genet 297</t>
-  </si>
-  <si>
-    <t>data sheet says genet 029, but it is genet 298</t>
-  </si>
-  <si>
-    <t>data sheet says genet 029, but it is genet 299</t>
-  </si>
-  <si>
-    <t>data sheet says genet 029, but it is genet 300</t>
-  </si>
-  <si>
-    <t>data sheet says genet 029, but it is genet 301</t>
-  </si>
-  <si>
-    <t>data sheet says genet 029, but it is genet 302</t>
-  </si>
-  <si>
-    <t>data sheet says genet 029, but it is genet 303</t>
-  </si>
-  <si>
-    <t>data sheet says genet 029, but it is genet 304</t>
-  </si>
-  <si>
-    <t>data sheet says genet 029, but it is genet 305</t>
-  </si>
-  <si>
-    <t>data sheet says genet 029, but it is genet 306</t>
-  </si>
-  <si>
-    <t>data sheet says genet 029, but it is genet 307</t>
-  </si>
-  <si>
-    <t>data sheet says genet 029, but it is genet 308</t>
   </si>
 </sst>
 </file>
@@ -542,8 +491,8 @@
   <dimension ref="A1:M145"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A125" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K145" sqref="K145"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N114" sqref="N114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4257,7 +4206,7 @@
         <v>29.2</v>
       </c>
     </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>13</v>
       </c>
@@ -4295,7 +4244,7 @@
         <v>29.2</v>
       </c>
     </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>13</v>
       </c>
@@ -4333,7 +4282,7 @@
         <v>29.8</v>
       </c>
     </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>13</v>
       </c>
@@ -4371,7 +4320,7 @@
         <v>29.8</v>
       </c>
     </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>13</v>
       </c>
@@ -4409,7 +4358,7 @@
         <v>29.7</v>
       </c>
     </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>13</v>
       </c>
@@ -4446,11 +4395,8 @@
       <c r="L101">
         <v>29.6</v>
       </c>
-      <c r="M101" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="102" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>13</v>
       </c>
@@ -4487,11 +4433,8 @@
       <c r="L102">
         <v>29.9</v>
       </c>
-      <c r="M102" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="103" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>13</v>
       </c>
@@ -4528,11 +4471,8 @@
       <c r="L103">
         <v>29.9</v>
       </c>
-      <c r="M103" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="104" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>13</v>
       </c>
@@ -4569,11 +4509,8 @@
       <c r="L104">
         <v>30.1</v>
       </c>
-      <c r="M104" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="105" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>13</v>
       </c>
@@ -4610,11 +4547,8 @@
       <c r="L105">
         <v>29.5</v>
       </c>
-      <c r="M105" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="106" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>13</v>
       </c>
@@ -4651,11 +4585,8 @@
       <c r="L106">
         <v>30.1</v>
       </c>
-      <c r="M106" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="107" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>13</v>
       </c>
@@ -4692,11 +4623,8 @@
       <c r="L107">
         <v>29.1</v>
       </c>
-      <c r="M107" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="108" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="108" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>13</v>
       </c>
@@ -4733,11 +4661,8 @@
       <c r="L108">
         <v>30.1</v>
       </c>
-      <c r="M108" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="109" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>13</v>
       </c>
@@ -4774,11 +4699,8 @@
       <c r="L109">
         <v>29.9</v>
       </c>
-      <c r="M109" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="110" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="110" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>13</v>
       </c>
@@ -4815,11 +4737,8 @@
       <c r="L110">
         <v>29.7</v>
       </c>
-      <c r="M110" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="111" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="111" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>13</v>
       </c>
@@ -4856,11 +4775,8 @@
       <c r="L111">
         <v>29.8</v>
       </c>
-      <c r="M111" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="112" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="112" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>13</v>
       </c>
@@ -4897,11 +4813,8 @@
       <c r="L112">
         <v>29.7</v>
       </c>
-      <c r="M112" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="113" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="113" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>13</v>
       </c>
@@ -4938,11 +4851,8 @@
       <c r="L113">
         <v>29.6</v>
       </c>
-      <c r="M113" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="114" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="114" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>13</v>
       </c>
@@ -4980,7 +4890,7 @@
         <v>29.6</v>
       </c>
     </row>
-    <row r="115" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>13</v>
       </c>
@@ -5018,7 +4928,7 @@
         <v>29.6</v>
       </c>
     </row>
-    <row r="116" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>13</v>
       </c>
@@ -5056,7 +4966,7 @@
         <v>29.5</v>
       </c>
     </row>
-    <row r="117" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>13</v>
       </c>
@@ -5094,7 +5004,7 @@
         <v>29.5</v>
       </c>
     </row>
-    <row r="118" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>13</v>
       </c>
@@ -5132,7 +5042,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="119" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>13</v>
       </c>
@@ -5170,7 +5080,7 @@
         <v>29.8</v>
       </c>
     </row>
-    <row r="120" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>13</v>
       </c>
@@ -5208,7 +5118,7 @@
         <v>29.7</v>
       </c>
     </row>
-    <row r="121" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>13</v>
       </c>
@@ -5246,7 +5156,7 @@
         <v>29.9</v>
       </c>
     </row>
-    <row r="122" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>13</v>
       </c>
@@ -5284,7 +5194,7 @@
         <v>29.8</v>
       </c>
     </row>
-    <row r="123" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>13</v>
       </c>
@@ -5322,7 +5232,7 @@
         <v>29.7</v>
       </c>
     </row>
-    <row r="124" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>13</v>
       </c>
@@ -5360,7 +5270,7 @@
         <v>29.6</v>
       </c>
     </row>
-    <row r="125" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>13</v>
       </c>
@@ -5398,7 +5308,7 @@
         <v>29.6</v>
       </c>
     </row>
-    <row r="126" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>13</v>
       </c>
@@ -5436,7 +5346,7 @@
         <v>29.3</v>
       </c>
     </row>
-    <row r="127" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>13</v>
       </c>
@@ -5474,7 +5384,7 @@
         <v>29.1</v>
       </c>
     </row>
-    <row r="128" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>13</v>
       </c>
@@ -5512,7 +5422,7 @@
         <v>29.5</v>
       </c>
     </row>
-    <row r="129" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>13</v>
       </c>
@@ -5550,7 +5460,7 @@
         <v>29.5</v>
       </c>
     </row>
-    <row r="130" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>13</v>
       </c>
@@ -5587,11 +5497,8 @@
       <c r="L130">
         <v>29.4</v>
       </c>
-      <c r="M130" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="131" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="131" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>13</v>
       </c>
@@ -5628,11 +5535,8 @@
       <c r="L131">
         <v>29.3</v>
       </c>
-      <c r="M131" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="132" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="132" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>13</v>
       </c>
@@ -5669,11 +5573,8 @@
       <c r="L132">
         <v>29.8</v>
       </c>
-      <c r="M132" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="133" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="133" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>13</v>
       </c>
@@ -5710,11 +5611,8 @@
       <c r="L133">
         <v>29.1</v>
       </c>
-      <c r="M133" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="134" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="134" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>13</v>
       </c>
@@ -5751,11 +5649,8 @@
       <c r="L134">
         <v>29.4</v>
       </c>
-      <c r="M134" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="135" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="135" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>13</v>
       </c>
@@ -5792,11 +5687,8 @@
       <c r="L135">
         <v>28.9</v>
       </c>
-      <c r="M135" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="136" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="136" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>13</v>
       </c>
@@ -5833,11 +5725,8 @@
       <c r="L136">
         <v>28.9</v>
       </c>
-      <c r="M136" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="137" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="137" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>13</v>
       </c>
@@ -5874,11 +5763,8 @@
       <c r="L137">
         <v>28.8</v>
       </c>
-      <c r="M137" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="138" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="138" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>13</v>
       </c>
@@ -5915,11 +5801,8 @@
       <c r="L138">
         <v>28.9</v>
       </c>
-      <c r="M138" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="139" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="139" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>13</v>
       </c>
@@ -5956,11 +5839,8 @@
       <c r="L139">
         <v>28.8</v>
       </c>
-      <c r="M139" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="140" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="140" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>13</v>
       </c>
@@ -5997,11 +5877,8 @@
       <c r="L140">
         <v>28.9</v>
       </c>
-      <c r="M140" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="141" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="141" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>13</v>
       </c>
@@ -6038,11 +5915,8 @@
       <c r="L141">
         <v>28.8</v>
       </c>
-      <c r="M141" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="142" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="142" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>13</v>
       </c>
@@ -6079,11 +5953,8 @@
       <c r="L142">
         <v>28.5</v>
       </c>
-      <c r="M142" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="143" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="143" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>13</v>
       </c>
@@ -6120,11 +5991,8 @@
       <c r="L143">
         <v>28.5</v>
       </c>
-      <c r="M143" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="144" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="144" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>13</v>
       </c>
@@ -6161,11 +6029,8 @@
       <c r="L144">
         <v>28.1</v>
       </c>
-      <c r="M144" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="145" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="145" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>13</v>
       </c>
@@ -6201,9 +6066,6 @@
       </c>
       <c r="L145">
         <v>28.9</v>
-      </c>
-      <c r="M145" t="s">
-        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>